<commit_message>
modification code CM et CS (#31)
modification code CM et CS #prolongee-prorogee => #prorogee 2b72fe3d4bab6496659a5d9d64360fdd45b6509f
</commit_message>
<xml_diff>
--- a/ig/main/CodeSystem-eclaire-study-status-code-system.xlsx
+++ b/ig/main/CodeSystem-eclaire-study-status-code-system.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-27T08:48:31+00:00</t>
+    <t>2023-07-27T13:16:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -147,10 +147,10 @@
     <t>Suspendue</t>
   </si>
   <si>
-    <t>prolongee-prorogee</t>
-  </si>
-  <si>
-    <t>Prolongée - prorogée</t>
+    <t>prorogee</t>
+  </si>
+  <si>
+    <t>Prorogée</t>
   </si>
   <si>
     <t>expiree</t>

</xml_diff>